<commit_message>
changes in the range of scores
</commit_message>
<xml_diff>
--- a/prep/CS_CP_HAB/hab_mangrove_trend_mse2019.xlsx
+++ b/prep/CS_CP_HAB/hab_mangrove_trend_mse2019.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Hurtadoyhurtado\carpeta compartida\PROYECTOS\CI IdSO MANABÍ Y SANTA ELENA\CAPAS DE DATOS\DATOS CRUDOS\BIODIVERSIDAD\HÁBITATS\DATOS CRUDOS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\karla\Documents\Github\mse\prep\CS_CP_HAB\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72BB1787-86E8-45DE-9BD5-7893C5226431}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19350" windowHeight="11760" activeTab="2"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19770" windowHeight="11760" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Manglar total mse" sheetId="5" r:id="rId1"/>
@@ -21,7 +22,7 @@
     <externalReference r:id="rId5"/>
     <externalReference r:id="rId6"/>
   </externalReferences>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +30,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -228,7 +231,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.000000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
@@ -447,7 +450,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -463,7 +466,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
@@ -477,7 +480,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -601,6 +603,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-8BE2-4E71-A28D-5D2964E8BD87}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -765,7 +772,7 @@
 </file>
 
 <file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
@@ -966,6 +973,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-EB84-41BA-B146-E6E6E2A23210}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1132,7 +1144,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
@@ -1146,7 +1158,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1270,6 +1281,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-1260-41E5-96CE-7E31C2F52573}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1434,7 +1450,7 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
@@ -1482,7 +1498,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1645,6 +1660,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-CEB3-4543-A806-B10CA1CBFC6D}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1811,7 +1831,7 @@
 </file>
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
@@ -1859,7 +1879,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2022,6 +2041,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-80D7-4543-AB18-780D90488F76}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -2188,7 +2212,7 @@
 </file>
 
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
@@ -2241,7 +2265,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2404,6 +2427,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-233D-4A12-A8B6-71B90216AE8A}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -2570,7 +2598,7 @@
 </file>
 
 <file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
@@ -2623,7 +2651,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2786,6 +2813,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-A865-47A1-9F28-ECB2DF45157B}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -2952,7 +2984,7 @@
 </file>
 
 <file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
@@ -2991,7 +3023,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3154,6 +3185,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-1BFB-432B-B706-B3ADA41ED735}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -3320,7 +3356,7 @@
 </file>
 
 <file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
@@ -3359,7 +3395,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3522,6 +3557,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-8611-4021-97E6-BB054BA10E5E}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -3688,7 +3728,7 @@
 </file>
 
 <file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
@@ -3894,6 +3934,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-AB1F-4E15-B53F-EFDD2A969A2A}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -8524,7 +8569,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Gráfico 1"/>
+        <xdr:cNvPr id="2" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -8556,7 +8607,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Gráfico 2"/>
+        <xdr:cNvPr id="3" name="Gráfico 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -8593,7 +8650,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="6" name="Gráfico 5"/>
+        <xdr:cNvPr id="6" name="Gráfico 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -8623,7 +8686,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="7" name="Gráfico 6"/>
+        <xdr:cNvPr id="7" name="Gráfico 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -8653,7 +8722,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="9" name="Gráfico 8"/>
+        <xdr:cNvPr id="9" name="Gráfico 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000009000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -8683,7 +8758,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="10" name="Gráfico 9"/>
+        <xdr:cNvPr id="10" name="Gráfico 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000A000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -8713,7 +8794,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="11" name="Gráfico 10"/>
+        <xdr:cNvPr id="11" name="Gráfico 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000B000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -8743,7 +8830,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="12" name="Gráfico 11"/>
+        <xdr:cNvPr id="12" name="Gráfico 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000C000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -8773,7 +8866,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="13" name="Gráfico 12"/>
+        <xdr:cNvPr id="13" name="Gráfico 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000D000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -8803,7 +8902,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="14" name="Gráfico 13"/>
+        <xdr:cNvPr id="14" name="Gráfico 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000E000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -9632,7 +9737,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R44"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -11166,7 +11271,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
@@ -11460,11 +11565,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11494,8 +11599,7 @@
         <v>2006</v>
       </c>
       <c r="D2">
-        <f>Cálculos!E8</f>
-        <v>-1.1494452149791956</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -11509,8 +11613,7 @@
         <v>2016</v>
       </c>
       <c r="D3">
-        <f>Cálculos!E9</f>
-        <v>-1.1248266296809988</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -11549,7 +11652,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>